<commit_message>
Fim de todo ETL, tabela de treimestre e comissões.
</commit_message>
<xml_diff>
--- a/Dados_forte_investimento.xlsx
+++ b/Dados_forte_investimento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70a760a74eefa2b5/Desktop/ProjetoPython/Projeto_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{87D07724-C505-4647-B481-8EFF40681C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D239A9-802F-4D20-8353-AED39E8370A9}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{87D07724-C505-4647-B481-8EFF40681C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F51AD7-389C-42A9-B114-B7A429FA3650}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D266C89-2A83-46B5-AA8F-22B5AB68DEA3}"/>
   </bookViews>
@@ -1143,6 +1143,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1477,24 +1481,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91783D3-CE3C-4289-8CDD-1DF2378C7F96}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I1" sqref="B1:I1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
     <col min="10" max="13" width="18.44140625" style="17" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
     <col min="15" max="15" width="26.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>